<commit_message>
Ajuste no algoritmo para considerar o preço de fechamento
</commit_message>
<xml_diff>
--- a/dados/MelhorCenario.xlsx
+++ b/dados/MelhorCenario.xlsx
@@ -577,12 +577,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.9987</t>
+          <t>0.9992</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.5642</t>
+          <t>0.5883</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -606,17 +606,17 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>R$ -452.57</t>
+          <t>R$ -375.97</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>R$ 252.48</t>
+          <t>R$ -17.93</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-04</t>
         </is>
       </c>
     </row>
@@ -658,12 +658,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.9963</t>
+          <t>0.9976</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.4400</t>
+          <t>0.4645</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -687,17 +687,17 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>R$ -308.05</t>
+          <t>R$ -330.90</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>R$ 654.64</t>
+          <t>R$ -71.70</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-16</t>
         </is>
       </c>
     </row>
@@ -739,12 +739,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.9929</t>
+          <t>0.9952</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.3613</t>
+          <t>0.3847</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>R$ -257.52</t>
+          <t>R$ -366.46</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>R$ 77.51</t>
+          <t>R$ -77.41</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -820,17 +820,17 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.9871</t>
+          <t>0.9911</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.2893</t>
+          <t>0.3107</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ITM → OTM</t>
+          <t>ITM → ATM</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -849,17 +849,17 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>R$ -239.02</t>
+          <t>R$ -363.35</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>R$ 34.03</t>
+          <t>R$ -69.38</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
     </row>
@@ -901,12 +901,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.9770</t>
+          <t>0.9843</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.1348</t>
+          <t>0.2447</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -923,19 +923,19 @@
         <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>252</v>
+        <v>30</v>
       </c>
       <c r="N6" t="n">
         <v>6</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>R$ -293.13</t>
+          <t>R$ -372.29</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>R$ 0.00</t>
+          <t>R$ -108.90</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -982,7 +982,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.5920</t>
+          <t>0.6628</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1004,24 +1004,24 @@
         <v>0.15</v>
       </c>
       <c r="M7" t="n">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>R$ 825.50</t>
+          <t>R$ 1051.01</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>R$ 1063.54</t>
+          <t>R$ 1051.01</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-06-10</t>
+          <t>2025-06-18</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.3832</t>
+          <t>0.4271</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1092,17 +1092,17 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>R$ 277.65</t>
+          <t>R$ 437.61</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>R$ 940.94</t>
+          <t>R$ 960.34</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-10</t>
         </is>
       </c>
     </row>
@@ -1144,12 +1144,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.3550</t>
+          <t>0.3690</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.9999</t>
+          <t>0.9982</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1166,19 +1166,19 @@
         <v>300</v>
       </c>
       <c r="M9" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="N9" t="n">
         <v>2</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>R$ 257.79</t>
+          <t>R$ 308.47</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>R$ 997.93</t>
+          <t>R$ 968.36</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.5104</t>
+          <t>0.5522</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1247,19 +1247,19 @@
         <v>300</v>
       </c>
       <c r="M10" t="n">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="N10" t="n">
         <v>2</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>R$ 1888.61</t>
+          <t>R$ 2047.65</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>R$ 1888.61</t>
+          <t>R$ 2047.65</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.2263</t>
+          <t>0.2569</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.7238</t>
+          <t>0.7320</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1335,12 +1335,12 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>R$ 404.12</t>
+          <t>R$ 590.57</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>R$ 564.99</t>
+          <t>R$ 724.28</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1387,12 +1387,12 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.1751</t>
+          <t>0.2016</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.1638</t>
+          <t>0.1700</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1416,17 +1416,17 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>R$ 477.52</t>
+          <t>R$ 713.64</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>R$ 565.94</t>
+          <t>R$ 713.64</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Criação dos boxplot para análise
</commit_message>
<xml_diff>
--- a/dados/MelhorCenario.xlsx
+++ b/dados/MelhorCenario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,12 +440,12 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="9" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
     <col width="11" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="7" customWidth="1" min="12" max="12"/>
-    <col width="22" customWidth="1" min="13" max="13"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
     <col width="11" customWidth="1" min="14" max="14"/>
     <col width="13" customWidth="1" min="15" max="15"/>
     <col width="14" customWidth="1" min="16" max="16"/>
@@ -490,12 +490,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>D.Inicial</t>
+          <t>Δ Inicio</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>D.Final</t>
+          <t>Δ Fim</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Pregões Volatilidade</t>
+          <t># Pregões Vol.</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -557,66 +557,66 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-25</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R$ 36.18</t>
+          <t>R$ 29.39</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R$ 29.45</t>
+          <t>R$ 30.09</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.9992</t>
+          <t>0.6078</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.5883</t>
+          <t>0.9859</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ITM → ATM</t>
+          <t>ATM → ITM</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>0.15</v>
       </c>
       <c r="M2" t="n">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="N2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>R$ -375.97</t>
+          <t>R$ 549.28</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>R$ -17.93</t>
+          <t>R$ 791.01</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-05-07</t>
         </is>
       </c>
     </row>
@@ -638,66 +638,66 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-25</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>R$ 36.18</t>
+          <t>R$ 29.39</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>R$ 29.45</t>
+          <t>R$ 30.09</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.9976</t>
+          <t>0.4832</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.4645</t>
+          <t>0.6469</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ITM → ATM</t>
+          <t>ATM → ATM</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Lote</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="M3" t="n">
         <v>30</v>
       </c>
       <c r="N3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>R$ -330.90</t>
+          <t>R$ 525.56</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>R$ -71.70</t>
+          <t>R$ 850.75</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-16</t>
+          <t>2025-05-07</t>
         </is>
       </c>
     </row>
@@ -719,66 +719,66 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-25</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>R$ 36.18</t>
+          <t>R$ 29.39</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>R$ 29.45</t>
+          <t>R$ 30.09</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.9952</t>
+          <t>0.4168</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.3847</t>
+          <t>0.3714</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ITM → ATM</t>
+          <t>ATM → ATM</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Lote</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="M4" t="n">
         <v>30</v>
       </c>
       <c r="N4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>R$ -366.46</t>
+          <t>R$ 578.41</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>R$ -77.41</t>
+          <t>R$ 793.28</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-05-07</t>
         </is>
       </c>
     </row>
@@ -800,66 +800,66 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-25</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>R$ 36.18</t>
+          <t>R$ 29.39</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R$ 29.45</t>
+          <t>R$ 30.09</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.9911</t>
+          <t>0.3536</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.3107</t>
+          <t>0.1535</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ITM → ATM</t>
+          <t>ATM → OTM</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="M5" t="n">
         <v>30</v>
       </c>
       <c r="N5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>R$ -363.35</t>
+          <t>R$ 834.81</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>R$ -69.38</t>
+          <t>R$ 835.13</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-05-08</t>
         </is>
       </c>
     </row>
@@ -881,66 +881,66 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-25</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>R$ 36.18</t>
+          <t>R$ 29.39</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>R$ 29.45</t>
+          <t>R$ 30.09</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.9843</t>
+          <t>0.2952</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.2447</t>
+          <t>0.0442</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ITM → OTM</t>
+          <t>OTM → OTM</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="M6" t="n">
         <v>30</v>
       </c>
       <c r="N6" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>R$ -372.29</t>
+          <t>R$ 986.22</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>R$ -108.90</t>
+          <t>R$ 986.22</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-05-15</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -972,17 +972,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.6628</t>
+          <t>0.7964</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -992,7 +992,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ATM → ITM</t>
+          <t>ITM → ITM</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1001,27 +1001,27 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="M7" t="n">
         <v>252</v>
       </c>
       <c r="N7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>R$ 1051.01</t>
+          <t>R$ 405.67</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>R$ 1051.01</t>
+          <t>R$ 532.66</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-06-18</t>
+          <t>2025-06-06</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1053,22 +1053,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.4271</t>
+          <t>0.5107</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.9999</t>
+          <t>0.9935</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1078,31 +1078,31 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Delta</t>
+          <t>Dias</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>60</v>
       </c>
       <c r="N8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>R$ 437.61</t>
+          <t>R$ -311.49</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>R$ 960.34</t>
+          <t>R$ 629.35</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-06-10</t>
+          <t>2025-06-06</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1134,22 +1134,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.3690</t>
+          <t>0.4405</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.9982</t>
+          <t>0.9505</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1159,26 +1159,26 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Lote</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>300</v>
+        <v>0.15</v>
       </c>
       <c r="M9" t="n">
         <v>60</v>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>R$ 308.47</t>
+          <t>R$ 20.74</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>R$ 968.36</t>
+          <t>R$ 531.67</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1215,17 +1215,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.5522</t>
+          <t>0.6334</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1240,26 +1240,26 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Lote</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>300</v>
+        <v>0.15</v>
       </c>
       <c r="M10" t="n">
-        <v>252</v>
+        <v>30</v>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>R$ 2047.65</t>
+          <t>R$ 699.60</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>R$ 2047.65</t>
+          <t>R$ 699.60</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1296,56 +1296,56 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.2569</t>
+          <t>0.2959</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.7320</t>
+          <t>0.1488</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>OTM → ITM</t>
+          <t>OTM → OTM</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Delta</t>
+          <t>Lote</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.15</v>
+        <v>300</v>
       </c>
       <c r="M11" t="n">
         <v>30</v>
       </c>
       <c r="N11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>R$ 590.57</t>
+          <t>R$ 509.95</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>R$ 724.28</t>
+          <t>R$ 509.95</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-18</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-05-02</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1377,22 +1377,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>R$ 29.32</t>
+          <t>R$ 30.22</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>R$ 32.96</t>
+          <t>R$ 32.23</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.2016</t>
+          <t>0.2288</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.1700</t>
+          <t>0.0045</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1402,31 +1402,1246 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Lote</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>300</v>
+        <v>0.15</v>
       </c>
       <c r="M12" t="n">
         <v>30</v>
       </c>
       <c r="N12" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>R$ 498.37</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>R$ 498.37</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PETRG307</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>R$ 29.23</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>R$ 31.66</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>R$ 31.07</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.8568</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.9999</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>ITM → ITM</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>200</v>
+      </c>
+      <c r="M13" t="n">
+        <v>60</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>R$ 807.41</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>R$ 807.41</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PETRG332</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>R$ 31.73</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>R$ 31.66</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>R$ 31.07</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.5656</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.0165</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>ATM → OTM</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>300</v>
+      </c>
+      <c r="M14" t="n">
+        <v>60</v>
+      </c>
+      <c r="N14" t="n">
+        <v>3</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>R$ 1364.07</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>R$ 1364.07</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PETRG353</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>R$ 30.98</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>R$ 31.66</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>R$ 31.07</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.6656</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.3324</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>ATM → ATM</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>300</v>
+      </c>
+      <c r="M15" t="n">
+        <v>60</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>R$ 1267.63</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>R$ 1267.63</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PETRG388</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>R$ 34.48</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>R$ 31.66</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>R$ 31.07</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0.2273</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>OTM → OTM</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>200</v>
+      </c>
+      <c r="M16" t="n">
+        <v>60</v>
+      </c>
+      <c r="N16" t="n">
+        <v>3</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>R$ 352.92</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>R$ 357.59</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PETRG398</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>R$ 35.48</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>R$ 31.66</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>R$ 31.07</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.0740</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>OTM → OTM</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Delta</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M17" t="n">
+        <v>30</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>R$ 234.10</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>R$ 308.51</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PETRH1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>R$ 35.23</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>R$ 31.52</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>R$ 30.05</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.1008</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>OTM → OTM</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>100</v>
+      </c>
+      <c r="M18" t="n">
+        <v>30</v>
+      </c>
+      <c r="N18" t="n">
+        <v>3</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>R$ 157.85</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>R$ 157.89</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PETRH335</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>R$ 31.98</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>R$ 31.52</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>R$ 30.05</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.5097</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>ATM → OTM</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Delta</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M19" t="n">
+        <v>252</v>
+      </c>
+      <c r="N19" t="n">
+        <v>4</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>R$ 762.73</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>R$ 828.27</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PETRH345</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>R$ 32.98</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>R$ 31.52</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>R$ 30.05</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.3489</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>ATM → OTM</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>300</v>
+      </c>
+      <c r="M20" t="n">
+        <v>30</v>
+      </c>
+      <c r="N20" t="n">
+        <v>3</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>R$ 623.22</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>R$ 648.72</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PETRH369</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>R$ 36.23</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>R$ 31.52</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>R$ 30.05</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.0340</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>OTM → OTM</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>7</v>
+      </c>
+      <c r="M21" t="n">
+        <v>60</v>
+      </c>
+      <c r="N21" t="n">
+        <v>5</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>R$ 71.73</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>R$ 71.73</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PETRI28</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>R$ 28.22</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.8163</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1.0000</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>ITM → ITM</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
         <v>1</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>R$ 713.64</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>R$ 713.64</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>2025-06-18</t>
+      <c r="M22" t="n">
+        <v>30</v>
+      </c>
+      <c r="N22" t="n">
+        <v>23</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>R$ 624.50</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>R$ 664.50</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PETRI288</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>R$ 27.47</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0.9027</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1.0000</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>ITM → ITM</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="n">
+        <v>30</v>
+      </c>
+      <c r="N23" t="n">
+        <v>23</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>R$ 462.30</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>R$ 462.30</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PETRI29</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>R$ 28.97</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0.6910</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1.0000</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>ATM → ITM</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
+        <v>60</v>
+      </c>
+      <c r="N24" t="n">
+        <v>23</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>R$ 466.71</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>R$ 506.71</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PETRI313</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>R$ 29.22</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0.6471</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>1.0000</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ATM → ITM</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>60</v>
+      </c>
+      <c r="N25" t="n">
+        <v>23</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>R$ 510.65</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>R$ 570.65</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PETRI333</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>R$ 31.22</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0.3191</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.6611</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>ATM → ATM</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Dias</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="n">
+        <v>120</v>
+      </c>
+      <c r="N26" t="n">
+        <v>23</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>R$ 749.88</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>R$ 749.88</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PETRI341</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>R$ 31.97</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>R$ 29.53</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>R$ 31.77</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0.2238</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.1502</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>OTM → OTM</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>100</v>
+      </c>
+      <c r="M27" t="n">
+        <v>120</v>
+      </c>
+      <c r="N27" t="n">
+        <v>3</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>R$ 658.49</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>R$ 706.12</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
         </is>
       </c>
     </row>

</xml_diff>